<commit_message>
Validation and Chnage password
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B358D0-399F-C440-87B3-1EB19913E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E22876-47FB-9641-BF50-E31F24691344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
   <dimension ref="B3:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Dashboard rename, Added Vehicle list screen
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/Services/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9284D281-01F5-A140-86CF-A32AC7B82143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCE44E2-E4EA-744C-B314-FFAA39F786DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ServicesList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="133">
   <si>
     <t>Services</t>
   </si>
@@ -415,6 +415,18 @@
   </si>
   <si>
     <t>/fileupload</t>
+  </si>
+  <si>
+    <t>Delete User Vehicle</t>
+  </si>
+  <si>
+    <t>WS-VS-04</t>
+  </si>
+  <si>
+    <t>app.vehicle.delete.uservehicle</t>
+  </si>
+  <si>
+    <t>/deletevehicle</t>
   </si>
 </sst>
 </file>
@@ -818,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
-  <dimension ref="B3:O29"/>
+  <dimension ref="B3:O30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,7 +914,7 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M18" si="0">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D4,"','CONNON_CONFIG', 0, '",C4,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M4:M19" si="0">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D4,"','CONNON_CONFIG', 0, '",C4,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-01','CONNON_CONFIG', 0, 'Refresh cache', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N4" t="str">
@@ -949,11 +961,11 @@
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-02','CONNON_CONFIG', 0, 'Refresh SQL', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N28" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
+        <f t="shared" ref="N5:N29" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
         <v>@PostMapping("/refreshsql")</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:O28" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
+        <f t="shared" ref="O5:O29" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-AP-02", serviceName = "Refresh SQL", queryId = "", logActivity =FALSE)</v>
       </c>
     </row>
@@ -1499,92 +1511,90 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="F18" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" t="str">
+        <f t="shared" ref="M18" si="6">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D18,"','CONNON_CONFIG', 0, '",C18,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-04','CONNON_CONFIG', 0, 'Delete User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" ref="N18" si="7">_xlfn.CONCAT(IF(I18="GET","@GetMapping(",IF(I18="POST","@PostMapping(",IF(I18="DELETE","@DeleteMapping(",IF(I18="PUT","@PutMapping(","")))),CHAR(34),H18,CHAR(34),")")</f>
+        <v>@DeleteMapping("/deletevehicle")</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" ref="O18" si="8">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D18,,CHAR(34),", serviceName = ",CHAR(34),C18,CHAR(34), ", queryId = ",CHAR(34),E18,CHAR(34),", logActivity =",F18,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-VS-04", serviceName = "Delete User Vehicle", queryId = "app.vehicle.delete.uservehicle", logActivity =TRUE)</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SE-01','CONNON_CONFIG', 0, 'Get All Active Services Types', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N18" t="str">
+      <c r="N19" t="str">
         <f t="shared" si="1"/>
         <v>@PostMapping("/type/all")</v>
       </c>
-      <c r="O18" t="str">
+      <c r="O19" t="str">
         <f t="shared" si="2"/>
         <v>@ServiceInfo(serviceCode = "WS-SE-01", serviceName = "Get All Active Services Types", queryId = "app.service.get.all", logActivity =FALSE)</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19" s="4"/>
-      <c r="M19" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D19,"','CONNON_CONFIG', 0, '",C19,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
@@ -1592,22 +1602,22 @@
         <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F20" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>16</v>
@@ -1616,20 +1626,20 @@
         <v>28</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" t="str">
-        <f t="shared" ref="M20:M28" si="6">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D20,"','CONNON_CONFIG', 0, '",C20,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D20,"','CONNON_CONFIG', 0, '",C20,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/create")</v>
+        <v>@PostMapping("/search")</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
@@ -1637,13 +1647,13 @@
         <v>66</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F21" s="4" t="b">
         <v>1</v>
@@ -1652,27 +1662,29 @@
         <v>70</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M21:M29" si="9">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D21,"','CONNON_CONFIG', 0, '",C21,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/update")</v>
+        <v>@PostMapping("/create")</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
@@ -1680,13 +1692,13 @@
         <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F22" s="4" t="b">
         <v>1</v>
@@ -1695,7 +1707,7 @@
         <v>70</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>81</v>
@@ -1706,16 +1718,16 @@
       </c>
       <c r="L22" s="4"/>
       <c r="M22" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/updatestatus")</v>
+        <v>@PutMapping("/update")</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
@@ -1723,13 +1735,13 @@
         <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F23" s="4" t="b">
         <v>1</v>
@@ -1738,10 +1750,10 @@
         <v>70</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="4" t="s">
@@ -1749,16 +1761,16 @@
       </c>
       <c r="L23" s="4"/>
       <c r="M23" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/delete")</v>
+        <v>@PutMapping("/updatestatus")</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
@@ -1766,13 +1778,13 @@
         <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F24" s="4" t="b">
         <v>1</v>
@@ -1781,29 +1793,27 @@
         <v>70</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J24" s="5"/>
       <c r="K24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/createrequest")</v>
+        <v>@DeleteMapping("/delete")</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
@@ -1811,13 +1821,13 @@
         <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F25" s="4" t="b">
         <v>1</v>
@@ -1826,27 +1836,29 @@
         <v>70</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/deleterequest")</v>
+        <v>@PostMapping("/createrequest")</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
@@ -1854,25 +1866,25 @@
         <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F26" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="4" t="s">
@@ -1880,16 +1892,16 @@
       </c>
       <c r="L26" s="4"/>
       <c r="M26" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequestcount")</v>
+        <v>@DeleteMapping("/deleterequest")</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
@@ -1897,13 +1909,13 @@
         <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F27" s="4" t="b">
         <v>0</v>
@@ -1912,7 +1924,7 @@
         <v>70</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>16</v>
@@ -1923,78 +1935,82 @@
       </c>
       <c r="L27" s="4"/>
       <c r="M27" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequest")</v>
+        <v>@PostMapping("/getrequestcount")</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F28" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J28" s="5"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L28" s="4"/>
       <c r="M28" t="str">
-        <f t="shared" si="6"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
+        <v>@PostMapping("/getrequest")</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="F29" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>16</v>
@@ -2003,20 +2019,59 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" t="str">
-        <f t="shared" ref="M29" si="7">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D29,"','CONNON_CONFIG', 0, '",C29,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" si="9"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/search")</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =FALSE)</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" t="str">
+        <f t="shared" ref="M30" si="10">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D30,"','CONNON_CONFIG', 0, '",C30,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-FL-01','CONNON_CONFIG', 0, 'File Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N29" t="str">
-        <f t="shared" ref="N29" si="8">_xlfn.CONCAT(IF(I29="GET","@GetMapping(",IF(I29="POST","@PostMapping(",IF(I29="DELETE","@DeleteMapping(",IF(I29="PUT","@PutMapping(","")))),CHAR(34),H29,CHAR(34),")")</f>
+      <c r="N30" t="str">
+        <f t="shared" ref="N30" si="11">_xlfn.CONCAT(IF(I30="GET","@GetMapping(",IF(I30="POST","@PostMapping(",IF(I30="DELETE","@DeleteMapping(",IF(I30="PUT","@PutMapping(","")))),CHAR(34),H30,CHAR(34),")")</f>
         <v>@PostMapping("/fileupload")</v>
       </c>
-      <c r="O29" t="str">
-        <f t="shared" ref="O29" si="9">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D29,,CHAR(34),", serviceName = ",CHAR(34),C29,CHAR(34), ", queryId = ",CHAR(34),E29,CHAR(34),", logActivity =",F29,")")</f>
+      <c r="O30" t="str">
+        <f t="shared" ref="O30" si="12">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D30,,CHAR(34),", serviceName = ",CHAR(34),C30,CHAR(34), ", queryId = ",CHAR(34),E30,CHAR(34),", logActivity =",F30,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =FALSE)</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:L28" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
+  <autoFilter ref="B3:L29" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add vehicle and My vehicle screen changes. Navigation changes.
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCE44E2-E4EA-744C-B314-FFAA39F786DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD11EFFC-B6D5-3249-B9DD-3E6BA8FA7E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ServicesList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="137">
   <si>
     <t>Services</t>
   </si>
@@ -427,6 +427,18 @@
   </si>
   <si>
     <t>/deletevehicle</t>
+  </si>
+  <si>
+    <t>Update User Vehicle</t>
+  </si>
+  <si>
+    <t>WS-VS-05</t>
+  </si>
+  <si>
+    <t>app.vehicle.update.uservehicle</t>
+  </si>
+  <si>
+    <t>/updatevehicle</t>
   </si>
 </sst>
 </file>
@@ -830,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
-  <dimension ref="B3:O30"/>
+  <dimension ref="B3:O31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +926,7 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M19" si="0">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D4,"','CONNON_CONFIG', 0, '",C4,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M4:M20" si="0">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D4,"','CONNON_CONFIG', 0, '",C4,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-01','CONNON_CONFIG', 0, 'Refresh cache', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N4" t="str">
@@ -961,11 +973,11 @@
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-02','CONNON_CONFIG', 0, 'Refresh SQL', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N29" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
+        <f t="shared" ref="N5:N30" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
         <v>@PostMapping("/refreshsql")</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:O29" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
+        <f t="shared" ref="O5:O30" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-AP-02", serviceName = "Refresh SQL", queryId = "", logActivity =FALSE)</v>
       </c>
     </row>
@@ -1554,92 +1566,90 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="F19" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" t="str">
+        <f t="shared" ref="M19" si="9">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D19,"','CONNON_CONFIG', 0, '",C19,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-05','CONNON_CONFIG', 0, 'Update User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" ref="N19" si="10">_xlfn.CONCAT(IF(I19="GET","@GetMapping(",IF(I19="POST","@PostMapping(",IF(I19="DELETE","@DeleteMapping(",IF(I19="PUT","@PutMapping(","")))),CHAR(34),H19,CHAR(34),")")</f>
+        <v>@PutMapping("/updatevehicle")</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" ref="O19" si="11">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D19,,CHAR(34),", serviceName = ",CHAR(34),C19,CHAR(34), ", queryId = ",CHAR(34),E19,CHAR(34),", logActivity =",F19,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-VS-05", serviceName = "Update User Vehicle", queryId = "app.vehicle.update.uservehicle", logActivity =TRUE)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SE-01','CONNON_CONFIG', 0, 'Get All Active Services Types', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N19" t="str">
+      <c r="N20" t="str">
         <f t="shared" si="1"/>
         <v>@PostMapping("/type/all")</v>
       </c>
-      <c r="O19" t="str">
+      <c r="O20" t="str">
         <f t="shared" si="2"/>
         <v>@ServiceInfo(serviceCode = "WS-SE-01", serviceName = "Get All Active Services Types", queryId = "app.service.get.all", logActivity =FALSE)</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" s="4"/>
-      <c r="M20" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D20,"','CONNON_CONFIG', 0, '",C20,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
@@ -1647,22 +1657,22 @@
         <v>66</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F21" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>16</v>
@@ -1671,20 +1681,20 @@
         <v>28</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" t="str">
-        <f t="shared" ref="M21:M29" si="9">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D21,"','CONNON_CONFIG', 0, '",C21,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D21,"','CONNON_CONFIG', 0, '",C21,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/create")</v>
+        <v>@PostMapping("/search")</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
@@ -1692,13 +1702,13 @@
         <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F22" s="4" t="b">
         <v>1</v>
@@ -1707,27 +1717,29 @@
         <v>70</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K22" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M22:M30" si="12">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D22,"','CONNON_CONFIG', 0, '",C22,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/update")</v>
+        <v>@PostMapping("/create")</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
@@ -1735,13 +1747,13 @@
         <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F23" s="4" t="b">
         <v>1</v>
@@ -1750,7 +1762,7 @@
         <v>70</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>81</v>
@@ -1761,16 +1773,16 @@
       </c>
       <c r="L23" s="4"/>
       <c r="M23" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/updatestatus")</v>
+        <v>@PutMapping("/update")</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
@@ -1778,13 +1790,13 @@
         <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F24" s="4" t="b">
         <v>1</v>
@@ -1793,10 +1805,10 @@
         <v>70</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="4" t="s">
@@ -1804,16 +1816,16 @@
       </c>
       <c r="L24" s="4"/>
       <c r="M24" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/delete")</v>
+        <v>@PutMapping("/updatestatus")</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
@@ -1821,13 +1833,13 @@
         <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F25" s="4" t="b">
         <v>1</v>
@@ -1836,29 +1848,27 @@
         <v>70</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J25" s="5"/>
       <c r="K25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/createrequest")</v>
+        <v>@DeleteMapping("/delete")</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
@@ -1866,13 +1876,13 @@
         <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -1881,27 +1891,29 @@
         <v>70</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/deleterequest")</v>
+        <v>@PostMapping("/createrequest")</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
@@ -1909,25 +1921,25 @@
         <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F27" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="4" t="s">
@@ -1935,16 +1947,16 @@
       </c>
       <c r="L27" s="4"/>
       <c r="M27" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequestcount")</v>
+        <v>@DeleteMapping("/deleterequest")</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =TRUE)</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
@@ -1952,13 +1964,13 @@
         <v>66</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F28" s="4" t="b">
         <v>0</v>
@@ -1967,7 +1979,7 @@
         <v>70</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>16</v>
@@ -1978,78 +1990,82 @@
       </c>
       <c r="L28" s="4"/>
       <c r="M28" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequest")</v>
+        <v>@PostMapping("/getrequestcount")</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F29" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J29" s="5"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
+        <v>@PostMapping("/getrequest")</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =FALSE)</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="F30" s="4" t="b">
         <v>0</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>16</v>
@@ -2058,20 +2074,59 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" t="str">
-        <f t="shared" ref="M30" si="10">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D30,"','CONNON_CONFIG', 0, '",C30,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" si="12"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/search")</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =FALSE)</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" t="str">
+        <f t="shared" ref="M31" si="13">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D31,"','CONNON_CONFIG', 0, '",C31,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-FL-01','CONNON_CONFIG', 0, 'File Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N30" t="str">
-        <f t="shared" ref="N30" si="11">_xlfn.CONCAT(IF(I30="GET","@GetMapping(",IF(I30="POST","@PostMapping(",IF(I30="DELETE","@DeleteMapping(",IF(I30="PUT","@PutMapping(","")))),CHAR(34),H30,CHAR(34),")")</f>
+      <c r="N31" t="str">
+        <f t="shared" ref="N31" si="14">_xlfn.CONCAT(IF(I31="GET","@GetMapping(",IF(I31="POST","@PostMapping(",IF(I31="DELETE","@DeleteMapping(",IF(I31="PUT","@PutMapping(","")))),CHAR(34),H31,CHAR(34),")")</f>
         <v>@PostMapping("/fileupload")</v>
       </c>
-      <c r="O30" t="str">
-        <f t="shared" ref="O30" si="12">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D30,,CHAR(34),", serviceName = ",CHAR(34),C30,CHAR(34), ", queryId = ",CHAR(34),E30,CHAR(34),", logActivity =",F30,")")</f>
+      <c r="O31" t="str">
+        <f t="shared" ref="O31" si="15">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D31,,CHAR(34),", serviceName = ",CHAR(34),C31,CHAR(34), ", queryId = ",CHAR(34),E31,CHAR(34),", logActivity =",F31,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =FALSE)</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:L29" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
+  <autoFilter ref="B3:L30" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
My Request screen changes.
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6C5B2B-24D7-274E-ACD1-E627C5BEE5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FF20CD-FEC5-8940-A9DC-59659AE85DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ServicesList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="150">
   <si>
     <t>Services</t>
   </si>
@@ -463,6 +463,21 @@
   </si>
   <si>
     <t>/profle</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Profile Update</t>
+  </si>
+  <si>
+    <t>WS-UP-11</t>
+  </si>
+  <si>
+    <t>app.user.profile.update</t>
   </si>
 </sst>
 </file>
@@ -539,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,6 +565,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -866,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
-  <dimension ref="B3:O33"/>
+  <dimension ref="B3:O34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,8 +951,8 @@
         <v>13</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2" t="b">
-        <v>0</v>
+      <c r="F4" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -950,7 +971,7 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M21" si="0">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D4,"','CONNON_CONFIG', 0, '",C4,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M4:M22" si="0">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D4,"','CONNON_CONFIG', 0, '",C4,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-01','CONNON_CONFIG', 0, 'Refresh cache', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N4" t="str">
@@ -959,7 +980,7 @@
       </c>
       <c r="O4" t="str">
         <f>_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D4,,CHAR(34),", serviceName = ",CHAR(34),C4,CHAR(34), ", queryId = ",CHAR(34),E4,CHAR(34),", logActivity =",F4,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-AP-01", serviceName = "Refresh cache", queryId = "", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-AP-01", serviceName = "Refresh cache", queryId = "", logActivity =false)</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
@@ -973,8 +994,8 @@
         <v>20</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
+      <c r="F5" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -997,12 +1018,12 @@
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-02','CONNON_CONFIG', 0, 'Refresh SQL', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N32" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
+        <f t="shared" ref="N5:N33" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
         <v>@PostMapping("/refreshsql")</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:O32" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-AP-02", serviceName = "Refresh SQL", queryId = "", logActivity =FALSE)</v>
+        <f t="shared" ref="O5:O33" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-AP-02", serviceName = "Refresh SQL", queryId = "", logActivity =false)</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
@@ -1018,8 +1039,8 @@
       <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="b">
-        <v>0</v>
+      <c r="F6" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>26</v>
@@ -1047,7 +1068,7 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-01", serviceName = "Get User Information", queryId = "app.user.get", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-01", serviceName = "Get User Information", queryId = "app.user.get", logActivity =false)</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1063,8 +1084,8 @@
       <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4" t="b">
-        <v>0</v>
+      <c r="F7" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>26</v>
@@ -1092,7 +1113,7 @@
       </c>
       <c r="O7" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-02", serviceName = "Get All User Information", queryId = "app.user.get.all", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-02", serviceName = "Get All User Information", queryId = "app.user.get.all", logActivity =false)</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
@@ -1108,8 +1129,8 @@
       <c r="E8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="4" t="b">
-        <v>1</v>
+      <c r="F8" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>26</v>
@@ -1137,7 +1158,7 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-03", serviceName = "User Registration", queryId = "app.user.save", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-03", serviceName = "User Registration", queryId = "app.user.save", logActivity =true)</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -1153,8 +1174,8 @@
       <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="4" t="b">
-        <v>1</v>
+      <c r="F9" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>26</v>
@@ -1182,7 +1203,7 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-04", serviceName = "Login service", queryId = "app.user.get", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-04", serviceName = "Login service", queryId = "app.user.get", logActivity =true)</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -1198,8 +1219,8 @@
       <c r="E10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="4" t="b">
-        <v>0</v>
+      <c r="F10" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>26</v>
@@ -1227,7 +1248,7 @@
       </c>
       <c r="O10" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-05", serviceName = "Logout service", queryId = "app.user.logout", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-05", serviceName = "Logout service", queryId = "app.user.logout", logActivity =false)</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
@@ -1243,8 +1264,8 @@
       <c r="E11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="4" t="b">
-        <v>0</v>
+      <c r="F11" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>26</v>
@@ -1272,7 +1293,7 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-06", serviceName = "User Type", queryId = "app.user.type.get", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-06", serviceName = "User Type", queryId = "app.user.type.get", logActivity =false)</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
@@ -1288,8 +1309,8 @@
       <c r="E12" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="4" t="b">
-        <v>1</v>
+      <c r="F12" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>26</v>
@@ -1317,7 +1338,7 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-07", serviceName = "Change Password", queryId = "app.user.password.update", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-07", serviceName = "Change Password", queryId = "app.user.password.update", logActivity =true)</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
@@ -1333,8 +1354,8 @@
       <c r="E13" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="4" t="b">
-        <v>1</v>
+      <c r="F13" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>26</v>
@@ -1362,7 +1383,7 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-UP-08", serviceName = "Forgot Password OTP", queryId = "app.user.otp.save", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-08", serviceName = "Forgot Password OTP", queryId = "app.user.otp.save", logActivity =true)</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
@@ -1378,8 +1399,8 @@
       <c r="E14" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="4" t="b">
-        <v>0</v>
+      <c r="F14" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>26</v>
@@ -1407,7 +1428,7 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" ref="O14" si="5">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D14,,CHAR(34),", serviceName = ",CHAR(34),C14,CHAR(34), ", queryId = ",CHAR(34),E14,CHAR(34),", logActivity =",F14,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-UP-09", serviceName = "Forgot Password validate OTP", queryId = "app.user.otp.get", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-09", serviceName = "Forgot Password validate OTP", queryId = "app.user.otp.get", logActivity =false)</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
@@ -1423,8 +1444,8 @@
       <c r="E15" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F15" s="4" t="b">
-        <v>0</v>
+      <c r="F15" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>26</v>
@@ -1438,7 +1459,9 @@
       <c r="J15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" t="str">
         <f t="shared" ref="M15" si="6">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D15,"','CONNON_CONFIG', 0, '",C15,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
@@ -1450,52 +1473,50 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" ref="O15" si="8">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D15,,CHAR(34),", serviceName = ",CHAR(34),C15,CHAR(34), ", queryId = ",CHAR(34),E15,CHAR(34),", logActivity =",F15,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-UP-10", serviceName = "Profile", queryId = "app.user.profile.get", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-UP-10", serviceName = "Profile", queryId = "app.user.profile.get", logActivity =false)</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="4" t="b">
-        <v>0</v>
+        <v>149</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-01','CONNON_CONFIG', 0, 'Get All Vehicle Types From Master', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M16" si="9">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D16,"','CONNON_CONFIG', 0, '",C16,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-UP-11','CONNON_CONFIG', 0, 'Profile Update', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/all")</v>
+        <f t="shared" ref="N16" si="10">_xlfn.CONCAT(IF(I16="GET","@GetMapping(",IF(I16="POST","@PostMapping(",IF(I16="DELETE","@DeleteMapping(",IF(I16="PUT","@PutMapping(","")))),CHAR(34),H16,CHAR(34),")")</f>
+        <v>@PutMapping("/profle")</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-VS-01", serviceName = "Get All Vehicle Types From Master", queryId = "app.vehicle.get.all", logActivity =FALSE)</v>
+        <f t="shared" ref="O16" si="11">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D16,,CHAR(34),", serviceName = ",CHAR(34),C16,CHAR(34), ", queryId = ",CHAR(34),E16,CHAR(34),", logActivity =",F16,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-UP-11", serviceName = "Profile Update", queryId = "app.user.profile.update", logActivity =true)</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
@@ -1503,22 +1524,22 @@
         <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="4" t="b">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>16</v>
@@ -1532,15 +1553,15 @@
       <c r="L17" s="4"/>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-02','CONNON_CONFIG', 0, 'User Vehicle Registration', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-01','CONNON_CONFIG', 0, 'Get All Vehicle Types From Master', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/registor")</v>
+        <v>@PostMapping("/all")</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-VS-02", serviceName = "User Vehicle Registration", queryId = "app.vehicle.save", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-VS-01", serviceName = "Get All Vehicle Types From Master", queryId = "app.vehicle.get.all", logActivity =false)</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
@@ -1548,22 +1569,22 @@
         <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="4" t="b">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>16</v>
@@ -1577,15 +1598,15 @@
       <c r="L18" s="4"/>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-03','CONNON_CONFIG', 0, 'Get User Vehicles', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-02','CONNON_CONFIG', 0, 'User Vehicle Registration', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/uservehicle")</v>
+        <v>@PostMapping("/registor")</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-VS-03", serviceName = "Get User Vehicles", queryId = "app.vehicle.get.uservehicle", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-VS-02", serviceName = "User Vehicle Registration", queryId = "app.vehicle.save", logActivity =true)</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
@@ -1593,42 +1614,44 @@
         <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="4" t="b">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L19" s="4"/>
       <c r="M19" t="str">
-        <f t="shared" ref="M19" si="9">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D19,"','CONNON_CONFIG', 0, '",C19,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-04','CONNON_CONFIG', 0, 'Delete User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-03','CONNON_CONFIG', 0, 'Get User Vehicles', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" ref="N19" si="10">_xlfn.CONCAT(IF(I19="GET","@GetMapping(",IF(I19="POST","@PostMapping(",IF(I19="DELETE","@DeleteMapping(",IF(I19="PUT","@PutMapping(","")))),CHAR(34),H19,CHAR(34),")")</f>
-        <v>@DeleteMapping("/deletevehicle")</v>
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/uservehicle")</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" ref="O19" si="11">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D19,,CHAR(34),", serviceName = ",CHAR(34),C19,CHAR(34), ", queryId = ",CHAR(34),E19,CHAR(34),", logActivity =",F19,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-VS-04", serviceName = "Delete User Vehicle", queryId = "app.vehicle.delete.uservehicle", logActivity =TRUE)</v>
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-VS-03", serviceName = "Get User Vehicles", queryId = "app.vehicle.get.uservehicle", logActivity =false)</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
@@ -1636,25 +1659,25 @@
         <v>48</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F20" s="4" t="b">
-        <v>1</v>
+        <v>131</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>28</v>
@@ -1663,105 +1686,103 @@
       <c r="L20" s="4"/>
       <c r="M20" t="str">
         <f t="shared" ref="M20" si="12">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D20,"','CONNON_CONFIG', 0, '",C20,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-05','CONNON_CONFIG', 0, 'Update User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-04','CONNON_CONFIG', 0, 'Delete User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" ref="N20" si="13">_xlfn.CONCAT(IF(I20="GET","@GetMapping(",IF(I20="POST","@PostMapping(",IF(I20="DELETE","@DeleteMapping(",IF(I20="PUT","@PutMapping(","")))),CHAR(34),H20,CHAR(34),")")</f>
-        <v>@PutMapping("/updatevehicle")</v>
+        <v>@DeleteMapping("/deletevehicle")</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" ref="O20" si="14">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D20,,CHAR(34),", serviceName = ",CHAR(34),C20,CHAR(34), ", queryId = ",CHAR(34),E20,CHAR(34),", logActivity =",F20,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-VS-05", serviceName = "Update User Vehicle", queryId = "app.vehicle.update.uservehicle", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-VS-04", serviceName = "Delete User Vehicle", queryId = "app.vehicle.delete.uservehicle", logActivity =true)</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="4" t="b">
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" t="str">
+        <f t="shared" ref="M21" si="15">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D21,"','CONNON_CONFIG', 0, '",C21,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-05','CONNON_CONFIG', 0, 'Update User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" ref="N21" si="16">_xlfn.CONCAT(IF(I21="GET","@GetMapping(",IF(I21="POST","@PostMapping(",IF(I21="DELETE","@DeleteMapping(",IF(I21="PUT","@PutMapping(","")))),CHAR(34),H21,CHAR(34),")")</f>
+        <v>@PutMapping("/updatevehicle")</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" ref="O21" si="17">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D21,,CHAR(34),", serviceName = ",CHAR(34),C21,CHAR(34), ", queryId = ",CHAR(34),E21,CHAR(34),", logActivity =",F21,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-VS-05", serviceName = "Update User Vehicle", queryId = "app.vehicle.update.uservehicle", logActivity =true)</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SE-01','CONNON_CONFIG', 0, 'Get All Active Services Types', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N21" t="str">
+      <c r="N22" t="str">
         <f t="shared" si="1"/>
         <v>@PostMapping("/type/all")</v>
       </c>
-      <c r="O21" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-SE-01", serviceName = "Get All Active Services Types", queryId = "app.service.get.all", logActivity =FALSE)</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L22" s="4"/>
-      <c r="M22" t="str">
-        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D22,"','CONNON_CONFIG', 0, '",C22,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
-      </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-SE-01", serviceName = "Get All Active Services Types", queryId = "app.service.get.all", logActivity =false)</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
@@ -1769,22 +1790,22 @@
         <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="4" t="b">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>16</v>
@@ -1793,20 +1814,20 @@
         <v>28</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" t="str">
-        <f t="shared" ref="M23:M32" si="15">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D23,"','CONNON_CONFIG', 0, '",C23,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D23,"','CONNON_CONFIG', 0, '",C23,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/create")</v>
+        <v>@PostMapping("/search")</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =false)</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
@@ -1814,42 +1835,44 @@
         <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="4" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J24" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M24:M33" si="18">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D24,"','CONNON_CONFIG', 0, '",C24,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/update")</v>
+        <v>@PostMapping("/create")</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =true)</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
@@ -1857,22 +1880,22 @@
         <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" s="4" t="b">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>81</v>
@@ -1883,16 +1906,16 @@
       </c>
       <c r="L25" s="4"/>
       <c r="M25" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/updatestatus")</v>
+        <v>@PutMapping("/update")</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =true)</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
@@ -1900,25 +1923,25 @@
         <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" s="4" t="b">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="4" t="s">
@@ -1926,16 +1949,16 @@
       </c>
       <c r="L26" s="4"/>
       <c r="M26" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/delete")</v>
+        <v>@PutMapping("/updatestatus")</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =true)</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
@@ -1943,44 +1966,42 @@
         <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="4" t="b">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J27" s="5"/>
       <c r="K27" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/createrequest")</v>
+        <v>@DeleteMapping("/delete")</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =true)</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
@@ -1988,42 +2009,44 @@
         <v>66</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="4" t="b">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K28" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/deleterequest")</v>
+        <v>@PostMapping("/createrequest")</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =TRUE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =true)</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
@@ -2031,25 +2054,25 @@
         <v>66</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="4" t="b">
-        <v>0</v>
+        <v>97</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="4" t="s">
@@ -2057,16 +2080,16 @@
       </c>
       <c r="L29" s="4"/>
       <c r="M29" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequestcount")</v>
+        <v>@DeleteMapping("/deleterequest")</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =true)</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
@@ -2074,22 +2097,22 @@
         <v>66</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" s="4" t="b">
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>16</v>
@@ -2100,16 +2123,16 @@
       </c>
       <c r="L30" s="4"/>
       <c r="M30" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequest")</v>
+        <v>@PostMapping("/getrequestcount")</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =FALSE)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =false)</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
@@ -2117,22 +2140,22 @@
         <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F31" s="4" t="b">
-        <v>0</v>
+        <v>105</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>70</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>16</v>
@@ -2143,78 +2166,82 @@
       </c>
       <c r="L31" s="4"/>
       <c r="M31" t="str">
-        <f t="shared" ref="M31" si="16">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D31,"','CONNON_CONFIG', 0, '",C31,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-10','CONNON_CONFIG', 0, 'Post Views', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" ref="N31" si="17">_xlfn.CONCAT(IF(I31="GET","@GetMapping(",IF(I31="POST","@PostMapping(",IF(I31="DELETE","@DeleteMapping(",IF(I31="PUT","@PutMapping(","")))),CHAR(34),H31,CHAR(34),")")</f>
-        <v>@PostMapping("/views")</v>
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/getrequest")</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" ref="O31" si="18">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D31,,CHAR(34),", serviceName = ",CHAR(34),C31,CHAR(34), ", queryId = ",CHAR(34),E31,CHAR(34),", logActivity =",F31,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-PS-10", serviceName = "Post Views", queryId = "app.post.save.viewe", logActivity =FALSE)</v>
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =false)</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" s="4" t="b">
-        <v>0</v>
+        <v>139</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="5"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L32" s="4"/>
       <c r="M32" t="str">
-        <f t="shared" si="15"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M32" si="19">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D32,"','CONNON_CONFIG', 0, '",C32,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-10','CONNON_CONFIG', 0, 'Post Views', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
+        <f t="shared" ref="N32" si="20">_xlfn.CONCAT(IF(I32="GET","@GetMapping(",IF(I32="POST","@PostMapping(",IF(I32="DELETE","@DeleteMapping(",IF(I32="PUT","@PutMapping(","")))),CHAR(34),H32,CHAR(34),")")</f>
+        <v>@PostMapping("/views")</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =FALSE)</v>
+        <f t="shared" ref="O32" si="21">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D32,,CHAR(34),", serviceName = ",CHAR(34),C32,CHAR(34), ", queryId = ",CHAR(34),E32,CHAR(34),", logActivity =",F32,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-PS-10", serviceName = "Post Views", queryId = "app.post.save.viewe", logActivity =false)</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4" t="b">
-        <v>0</v>
+        <v>109</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>16</v>
@@ -2223,20 +2250,59 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" t="str">
-        <f t="shared" ref="M33" si="19">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D33,"','CONNON_CONFIG', 0, '",C33,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" si="18"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/search")</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =false)</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" t="str">
+        <f t="shared" ref="M34" si="22">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D34,"','CONNON_CONFIG', 0, '",C34,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-FL-01','CONNON_CONFIG', 0, 'File Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N33" t="str">
-        <f t="shared" ref="N33" si="20">_xlfn.CONCAT(IF(I33="GET","@GetMapping(",IF(I33="POST","@PostMapping(",IF(I33="DELETE","@DeleteMapping(",IF(I33="PUT","@PutMapping(","")))),CHAR(34),H33,CHAR(34),")")</f>
+      <c r="N34" t="str">
+        <f t="shared" ref="N34" si="23">_xlfn.CONCAT(IF(I34="GET","@GetMapping(",IF(I34="POST","@PostMapping(",IF(I34="DELETE","@DeleteMapping(",IF(I34="PUT","@PutMapping(","")))),CHAR(34),H34,CHAR(34),")")</f>
         <v>@PostMapping("/fileupload")</v>
       </c>
-      <c r="O33" t="str">
-        <f t="shared" ref="O33" si="21">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D33,,CHAR(34),", serviceName = ",CHAR(34),C33,CHAR(34), ", queryId = ",CHAR(34),E33,CHAR(34),", logActivity =",F33,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =FALSE)</v>
+      <c r="O34" t="str">
+        <f t="shared" ref="O34" si="24">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D34,,CHAR(34),", serviceName = ",CHAR(34),C34,CHAR(34), ", queryId = ",CHAR(34),E34,CHAR(34),", logActivity =",F34,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =false)</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:L32" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
+  <autoFilter ref="B3:L34" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create different post search api for customer and service provider.
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8841C1-9B55-4749-83D2-E8B2BA2F303C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C015C14-40AD-D840-9180-3E2D3516CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ServicesList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="154">
   <si>
     <t>Services</t>
   </si>
@@ -231,15 +231,9 @@
     <t>Post</t>
   </si>
   <si>
-    <t>Search post</t>
-  </si>
-  <si>
     <t>WS-PS-01</t>
   </si>
   <si>
-    <t>app.post.search</t>
-  </si>
-  <si>
     <t>post</t>
   </si>
   <si>
@@ -478,6 +472,24 @@
   </si>
   <si>
     <t>app.user.profile.update</t>
+  </si>
+  <si>
+    <t>Search post Customer</t>
+  </si>
+  <si>
+    <t>Search post Service Provider</t>
+  </si>
+  <si>
+    <t>app.post.search.customer</t>
+  </si>
+  <si>
+    <t>app.post.search.provider</t>
+  </si>
+  <si>
+    <t>/search-customer</t>
+  </si>
+  <si>
+    <t>/search-provider</t>
   </si>
 </sst>
 </file>
@@ -887,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
-  <dimension ref="B3:O34"/>
+  <dimension ref="B3:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,7 +964,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -995,7 +1007,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -1018,11 +1030,11 @@
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-AP-02','CONNON_CONFIG', 0, 'Refresh SQL', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N33" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
+        <f t="shared" ref="N5:N34" si="1">_xlfn.CONCAT(IF(I5="GET","@GetMapping(",IF(I5="POST","@PostMapping(",IF(I5="DELETE","@DeleteMapping(",IF(I5="PUT","@PutMapping(","")))),CHAR(34),H5,CHAR(34),")")</f>
         <v>@PostMapping("/refreshsql")</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:O33" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
+        <f t="shared" ref="O5:O34" si="2">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D5,,CHAR(34),", serviceName = ",CHAR(34),C5,CHAR(34), ", queryId = ",CHAR(34),E5,CHAR(34),", logActivity =",F5,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-AP-02", serviceName = "Refresh SQL", queryId = "", logActivity =false)</v>
       </c>
     </row>
@@ -1040,7 +1052,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>26</v>
@@ -1085,7 +1097,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>26</v>
@@ -1130,7 +1142,7 @@
         <v>35</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>26</v>
@@ -1175,7 +1187,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>26</v>
@@ -1220,7 +1232,7 @@
         <v>42</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>26</v>
@@ -1265,7 +1277,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>26</v>
@@ -1301,31 +1313,31 @@
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" t="str">
@@ -1346,22 +1358,22 @@
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>16</v>
@@ -1370,7 +1382,7 @@
         <v>28</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" t="str">
@@ -1391,22 +1403,22 @@
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>16</v>
@@ -1415,7 +1427,7 @@
         <v>28</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" t="str">
@@ -1436,22 +1448,22 @@
         <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>16</v>
@@ -1460,7 +1472,7 @@
         <v>28</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" t="str">
@@ -1481,25 +1493,25 @@
         <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="F16" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>28</v>
@@ -1533,7 +1545,7 @@
         <v>51</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>52</v>
@@ -1578,7 +1590,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>52</v>
@@ -1623,7 +1635,7 @@
         <v>58</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>52</v>
@@ -1659,25 +1671,25 @@
         <v>48</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>28</v>
@@ -1702,25 +1714,25 @@
         <v>48</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>28</v>
@@ -1754,7 +1766,7 @@
         <v>63</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>64</v>
@@ -1790,22 +1802,22 @@
         <v>66</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="H23" s="4" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>16</v>
@@ -1814,20 +1826,20 @@
         <v>28</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D23,"','CONNON_CONFIG', 0, '",C23,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post Customer', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
+        <v>@PostMapping("/search-customer")</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post", queryId = "app.post.search", logActivity =false)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post Customer", queryId = "app.post.search.customer", logActivity =false)</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
@@ -1835,22 +1847,22 @@
         <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>16</v>
@@ -1859,20 +1871,20 @@
         <v>28</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" t="str">
-        <f t="shared" ref="M24:M33" si="18">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D24,"','CONNON_CONFIG', 0, '",C24,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D24,"','CONNON_CONFIG', 0, '",C24,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post Service Provider', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/create")</v>
+        <f t="shared" ref="N24" si="18">_xlfn.CONCAT(IF(I24="GET","@GetMapping(",IF(I24="POST","@PostMapping(",IF(I24="DELETE","@DeleteMapping(",IF(I24="PUT","@PutMapping(","")))),CHAR(34),H24,CHAR(34),")")</f>
+        <v>@PostMapping("/search-provider")</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =true)</v>
+        <f t="shared" ref="O24" si="19">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D24,,CHAR(34),", serviceName = ",CHAR(34),C24,CHAR(34), ", queryId = ",CHAR(34),E24,CHAR(34),", logActivity =",F24,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post Service Provider", queryId = "app.post.search.provider", logActivity =false)</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
@@ -1880,42 +1892,44 @@
         <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J25" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M25:M34" si="20">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D25,"','CONNON_CONFIG', 0, '",C25,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/update")</v>
+        <v>@PostMapping("/create")</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =true)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-02", serviceName = "Create Post", queryId = "app.post.create", logActivity =true)</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
@@ -1923,25 +1937,25 @@
         <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="4" t="s">
@@ -1949,16 +1963,16 @@
       </c>
       <c r="L26" s="4"/>
       <c r="M26" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="1"/>
-        <v>@PutMapping("/updatestatus")</v>
+        <v>@PutMapping("/update")</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =true)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-03", serviceName = "Update Post", queryId = "app.post.update", logActivity =true)</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
@@ -1966,25 +1980,25 @@
         <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="4" t="s">
@@ -1992,16 +2006,16 @@
       </c>
       <c r="L27" s="4"/>
       <c r="M27" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/delete")</v>
+        <v>@PutMapping("/updatestatus")</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =true)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-04", serviceName = "Update Post Status", queryId = "app.post.update.status", logActivity =true)</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
@@ -2009,44 +2023,42 @@
         <v>66</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J28" s="5"/>
       <c r="K28" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/createrequest")</v>
+        <v>@DeleteMapping("/delete")</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =true)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-05", serviceName = "Delete Post", queryId = "app.post.delete", logActivity =true)</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
@@ -2054,42 +2066,44 @@
         <v>66</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K29" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="1"/>
-        <v>@DeleteMapping("/deleterequest")</v>
+        <v>@PostMapping("/createrequest")</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =true)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-06", serviceName = "Create Post Request", queryId = "app.post.create.request", logActivity =true)</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
@@ -2097,25 +2111,25 @@
         <v>66</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="4" t="s">
@@ -2123,16 +2137,16 @@
       </c>
       <c r="L30" s="4"/>
       <c r="M30" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequestcount")</v>
+        <v>@DeleteMapping("/deleterequest")</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =false)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-07", serviceName = "Delete Post Request", queryId = "app.post.delete.request", logActivity =true)</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
@@ -2140,22 +2154,22 @@
         <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>16</v>
@@ -2166,16 +2180,16 @@
       </c>
       <c r="L31" s="4"/>
       <c r="M31" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="1"/>
-        <v>@PostMapping("/getrequest")</v>
+        <v>@PostMapping("/getrequestcount")</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =false)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-08", serviceName = "Get Post Request Count", queryId = "app.post.get.request.count", logActivity =false)</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
@@ -2183,22 +2197,22 @@
         <v>66</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>16</v>
@@ -2209,78 +2223,82 @@
       </c>
       <c r="L32" s="4"/>
       <c r="M32" t="str">
-        <f t="shared" ref="M32" si="19">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D32,"','CONNON_CONFIG', 0, '",C32,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-10','CONNON_CONFIG', 0, 'Post Views', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" ref="N32" si="20">_xlfn.CONCAT(IF(I32="GET","@GetMapping(",IF(I32="POST","@PostMapping(",IF(I32="DELETE","@DeleteMapping(",IF(I32="PUT","@PutMapping(","")))),CHAR(34),H32,CHAR(34),")")</f>
-        <v>@PostMapping("/views")</v>
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/getrequest")</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" ref="O32" si="21">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D32,,CHAR(34),", serviceName = ",CHAR(34),C32,CHAR(34), ", queryId = ",CHAR(34),E32,CHAR(34),", logActivity =",F32,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-PS-10", serviceName = "Post Views", queryId = "app.post.save.viewe", logActivity =false)</v>
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-PS-09", serviceName = "Get Post Request", queryId = "app.post.get.request", logActivity =false)</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J33" s="5"/>
-      <c r="K33" s="4"/>
+      <c r="K33" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L33" s="4"/>
       <c r="M33" t="str">
-        <f t="shared" si="18"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M33" si="21">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D33,"','CONNON_CONFIG', 0, '",C33,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-10','CONNON_CONFIG', 0, 'Post Views', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/search")</v>
+        <f t="shared" ref="N33" si="22">_xlfn.CONCAT(IF(I33="GET","@GetMapping(",IF(I33="POST","@PostMapping(",IF(I33="DELETE","@DeleteMapping(",IF(I33="PUT","@PutMapping(","")))),CHAR(34),H33,CHAR(34),")")</f>
+        <v>@PostMapping("/views")</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =false)</v>
+        <f t="shared" ref="O33" si="23">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D33,,CHAR(34),", serviceName = ",CHAR(34),C33,CHAR(34), ", queryId = ",CHAR(34),E33,CHAR(34),", logActivity =",F33,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-PS-10", serviceName = "Post Views", queryId = "app.post.save.viewe", logActivity =false)</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E34" s="4"/>
+        <v>107</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F34" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>16</v>
@@ -2289,20 +2307,59 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" t="str">
-        <f t="shared" ref="M34" si="22">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D34,"','CONNON_CONFIG', 0, '",C34,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" si="20"/>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="1"/>
+        <v>@PostMapping("/search")</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="2"/>
+        <v>@ServiceInfo(serviceCode = "WS-SP-01", serviceName = "Search Service Provider For Post", queryId = "app.serviceprovider.search", logActivity =false)</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" t="str">
+        <f t="shared" ref="M35" si="24">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D35,"','CONNON_CONFIG', 0, '",C35,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-FL-01','CONNON_CONFIG', 0, 'File Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
-      <c r="N34" t="str">
-        <f t="shared" ref="N34" si="23">_xlfn.CONCAT(IF(I34="GET","@GetMapping(",IF(I34="POST","@PostMapping(",IF(I34="DELETE","@DeleteMapping(",IF(I34="PUT","@PutMapping(","")))),CHAR(34),H34,CHAR(34),")")</f>
+      <c r="N35" t="str">
+        <f t="shared" ref="N35" si="25">_xlfn.CONCAT(IF(I35="GET","@GetMapping(",IF(I35="POST","@PostMapping(",IF(I35="DELETE","@DeleteMapping(",IF(I35="PUT","@PutMapping(","")))),CHAR(34),H35,CHAR(34),")")</f>
         <v>@PostMapping("/fileupload")</v>
       </c>
-      <c r="O34" t="str">
-        <f t="shared" ref="O34" si="24">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D34,,CHAR(34),", serviceName = ",CHAR(34),C34,CHAR(34), ", queryId = ",CHAR(34),E34,CHAR(34),", logActivity =",F34,")")</f>
+      <c r="O35" t="str">
+        <f t="shared" ref="O35" si="26">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D35,,CHAR(34),", serviceName = ",CHAR(34),C35,CHAR(34), ", queryId = ",CHAR(34),E35,CHAR(34),", logActivity =",F35,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =false)</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:L34" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
+  <autoFilter ref="B3:L35" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Image upload in Add vehicle screen.
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C015C14-40AD-D840-9180-3E2D3516CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBB552B-0213-A248-9CDC-964A6093A98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="159">
   <si>
     <t>Services</t>
   </si>
@@ -490,6 +490,21 @@
   </si>
   <si>
     <t>/search-provider</t>
+  </si>
+  <si>
+    <t>WS-PS-01-2</t>
+  </si>
+  <si>
+    <t>Image Upload</t>
+  </si>
+  <si>
+    <t>WS-IMG-01</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>/image</t>
   </si>
 </sst>
 </file>
@@ -899,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
-  <dimension ref="B3:O35"/>
+  <dimension ref="B3:O36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1850,7 +1865,7 @@
         <v>149</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>151</v>
@@ -1876,7 +1891,7 @@
       <c r="L24" s="4"/>
       <c r="M24" t="str">
         <f>_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D24,"','CONNON_CONFIG', 0, '",C24,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01','CONNON_CONFIG', 0, 'Search post Service Provider', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01-2','CONNON_CONFIG', 0, 'Search post Service Provider', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" ref="N24" si="18">_xlfn.CONCAT(IF(I24="GET","@GetMapping(",IF(I24="POST","@PostMapping(",IF(I24="DELETE","@DeleteMapping(",IF(I24="PUT","@PutMapping(","")))),CHAR(34),H24,CHAR(34),")")</f>
@@ -1884,7 +1899,7 @@
       </c>
       <c r="O24" t="str">
         <f t="shared" ref="O24" si="19">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D24,,CHAR(34),", serviceName = ",CHAR(34),C24,CHAR(34), ", queryId = ",CHAR(34),E24,CHAR(34),", logActivity =",F24,")")</f>
-        <v>@ServiceInfo(serviceCode = "WS-PS-01", serviceName = "Search post Service Provider", queryId = "app.post.search.provider", logActivity =false)</v>
+        <v>@ServiceInfo(serviceCode = "WS-PS-01-2", serviceName = "Search post Service Provider", queryId = "app.post.search.provider", logActivity =false)</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
@@ -2358,6 +2373,45 @@
         <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =false)</v>
       </c>
     </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" t="str">
+        <f t="shared" ref="M36" si="27">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D36,"','CONNON_CONFIG', 0, '",C36,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-IMG-01','CONNON_CONFIG', 0, 'Image Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" ref="N36" si="28">_xlfn.CONCAT(IF(I36="GET","@GetMapping(",IF(I36="POST","@PostMapping(",IF(I36="DELETE","@DeleteMapping(",IF(I36="PUT","@PutMapping(","")))),CHAR(34),H36,CHAR(34),")")</f>
+        <v>@PostMapping("/image")</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" ref="O36" si="29">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D36,,CHAR(34),", serviceName = ",CHAR(34),C36,CHAR(34), ", queryId = ",CHAR(34),E36,CHAR(34),", logActivity =",F36,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-IMG-01", serviceName = "Image Upload", queryId = "", logActivity =false)</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B3:L35" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Change password api added
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8701BE08-7B41-9944-AC7C-9136E4546733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C543655-687E-8F45-B892-3129077E5A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="165">
   <si>
     <t>Services</t>
   </si>
@@ -177,15 +177,6 @@
     <t>Vehicle</t>
   </si>
   <si>
-    <t>Get All Vehicle Types From Master</t>
-  </si>
-  <si>
-    <t>WS-VS-01</t>
-  </si>
-  <si>
-    <t>app.vehicle.get.all</t>
-  </si>
-  <si>
     <t>vehicle</t>
   </si>
   <si>
@@ -520,6 +511,18 @@
   </si>
   <si>
     <t>bid</t>
+  </si>
+  <si>
+    <t>Set New Password</t>
+  </si>
+  <si>
+    <t>WS-UP-12</t>
+  </si>
+  <si>
+    <t>app.user.password.setnew</t>
+  </si>
+  <si>
+    <t>/setnewpassword</t>
   </si>
 </sst>
 </file>
@@ -932,8 +935,8 @@
   <dimension ref="B3:O37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,7 +998,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -1038,7 +1041,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -1083,7 +1086,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>26</v>
@@ -1128,7 +1131,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>26</v>
@@ -1173,7 +1176,7 @@
         <v>35</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>26</v>
@@ -1218,7 +1221,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>26</v>
@@ -1263,7 +1266,7 @@
         <v>42</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>26</v>
@@ -1308,7 +1311,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>26</v>
@@ -1344,31 +1347,31 @@
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="F12" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" t="str">
@@ -1389,22 +1392,22 @@
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>16</v>
@@ -1413,7 +1416,7 @@
         <v>28</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" t="str">
@@ -1434,22 +1437,22 @@
         <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>16</v>
@@ -1458,7 +1461,7 @@
         <v>28</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" t="str">
@@ -1479,22 +1482,22 @@
         <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>16</v>
@@ -1503,7 +1506,7 @@
         <v>28</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" t="str">
@@ -1524,25 +1527,25 @@
         <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>28</v>
@@ -1564,47 +1567,45 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-01','CONNON_CONFIG', 0, 'Get All Vehicle Types From Master', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+        <f t="shared" ref="M17" si="12">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D17,"','CONNON_CONFIG', 0, '",C17,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-UP-12','CONNON_CONFIG', 0, 'Set New Password', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="1"/>
-        <v>@PostMapping("/all")</v>
+        <f t="shared" ref="N17" si="13">_xlfn.CONCAT(IF(I17="GET","@GetMapping(",IF(I17="POST","@PostMapping(",IF(I17="DELETE","@DeleteMapping(",IF(I17="PUT","@PutMapping(","")))),CHAR(34),H17,CHAR(34),")")</f>
+        <v>@PutMapping("/setnewpassword")</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" si="2"/>
-        <v>@ServiceInfo(serviceCode = "WS-VS-01", serviceName = "Get All Vehicle Types From Master", queryId = "app.vehicle.get.all", logActivity =false)</v>
+        <f t="shared" ref="O17" si="14">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D17,,CHAR(34),", serviceName = ",CHAR(34),C17,CHAR(34), ", queryId = ",CHAR(34),E17,CHAR(34),", logActivity =",F17,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-UP-12", serviceName = "Set New Password", queryId = "app.user.password.setnew", logActivity =true)</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
@@ -1612,19 +1613,19 @@
         <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>36</v>
@@ -1657,22 +1658,22 @@
         <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>16</v>
@@ -1702,25 +1703,25 @@
         <v>48</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="I20" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>28</v>
@@ -1728,15 +1729,15 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" t="str">
-        <f t="shared" ref="M20" si="12">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D20,"','CONNON_CONFIG', 0, '",C20,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M20" si="15">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D20,"','CONNON_CONFIG', 0, '",C20,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-04','CONNON_CONFIG', 0, 'Delete User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" ref="N20" si="13">_xlfn.CONCAT(IF(I20="GET","@GetMapping(",IF(I20="POST","@PostMapping(",IF(I20="DELETE","@DeleteMapping(",IF(I20="PUT","@PutMapping(","")))),CHAR(34),H20,CHAR(34),")")</f>
+        <f t="shared" ref="N20" si="16">_xlfn.CONCAT(IF(I20="GET","@GetMapping(",IF(I20="POST","@PostMapping(",IF(I20="DELETE","@DeleteMapping(",IF(I20="PUT","@PutMapping(","")))),CHAR(34),H20,CHAR(34),")")</f>
         <v>@DeleteMapping("/deletevehicle")</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" ref="O20" si="14">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D20,,CHAR(34),", serviceName = ",CHAR(34),C20,CHAR(34), ", queryId = ",CHAR(34),E20,CHAR(34),", logActivity =",F20,")")</f>
+        <f t="shared" ref="O20" si="17">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D20,,CHAR(34),", serviceName = ",CHAR(34),C20,CHAR(34), ", queryId = ",CHAR(34),E20,CHAR(34),", logActivity =",F20,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-VS-04", serviceName = "Delete User Vehicle", queryId = "app.vehicle.delete.uservehicle", logActivity =true)</v>
       </c>
     </row>
@@ -1745,25 +1746,25 @@
         <v>48</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="I21" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>28</v>
@@ -1771,39 +1772,39 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" t="str">
-        <f t="shared" ref="M21" si="15">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D21,"','CONNON_CONFIG', 0, '",C21,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M21" si="18">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D21,"','CONNON_CONFIG', 0, '",C21,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-VS-05','CONNON_CONFIG', 0, 'Update User Vehicle', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" ref="N21" si="16">_xlfn.CONCAT(IF(I21="GET","@GetMapping(",IF(I21="POST","@PostMapping(",IF(I21="DELETE","@DeleteMapping(",IF(I21="PUT","@PutMapping(","")))),CHAR(34),H21,CHAR(34),")")</f>
+        <f t="shared" ref="N21" si="19">_xlfn.CONCAT(IF(I21="GET","@GetMapping(",IF(I21="POST","@PostMapping(",IF(I21="DELETE","@DeleteMapping(",IF(I21="PUT","@PutMapping(","")))),CHAR(34),H21,CHAR(34),")")</f>
         <v>@PutMapping("/updatevehicle")</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" ref="O21" si="17">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D21,,CHAR(34),", serviceName = ",CHAR(34),C21,CHAR(34), ", queryId = ",CHAR(34),E21,CHAR(34),", logActivity =",F21,")")</f>
+        <f t="shared" ref="O21" si="20">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D21,,CHAR(34),", serviceName = ",CHAR(34),C21,CHAR(34), ", queryId = ",CHAR(34),E21,CHAR(34),", logActivity =",F21,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-VS-05", serviceName = "Update User Vehicle", queryId = "app.vehicle.update.uservehicle", logActivity =true)</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="F22" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>16</v>
@@ -1830,25 +1831,25 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>16</v>
@@ -1857,7 +1858,7 @@
         <v>28</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" t="str">
@@ -1875,25 +1876,25 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>16</v>
@@ -1902,7 +1903,7 @@
         <v>28</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" t="str">
@@ -1910,35 +1911,35 @@
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-01-2','CONNON_CONFIG', 0, 'Search post Service Provider', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" ref="N24" si="18">_xlfn.CONCAT(IF(I24="GET","@GetMapping(",IF(I24="POST","@PostMapping(",IF(I24="DELETE","@DeleteMapping(",IF(I24="PUT","@PutMapping(","")))),CHAR(34),H24,CHAR(34),")")</f>
+        <f t="shared" ref="N24" si="21">_xlfn.CONCAT(IF(I24="GET","@GetMapping(",IF(I24="POST","@PostMapping(",IF(I24="DELETE","@DeleteMapping(",IF(I24="PUT","@PutMapping(","")))),CHAR(34),H24,CHAR(34),")")</f>
         <v>@PostMapping("/search-provider")</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" ref="O24" si="19">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D24,,CHAR(34),", serviceName = ",CHAR(34),C24,CHAR(34), ", queryId = ",CHAR(34),E24,CHAR(34),", logActivity =",F24,")")</f>
+        <f t="shared" ref="O24" si="22">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D24,,CHAR(34),", serviceName = ",CHAR(34),C24,CHAR(34), ", queryId = ",CHAR(34),E24,CHAR(34),", logActivity =",F24,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-PS-01-2", serviceName = "Search post Service Provider", queryId = "app.post.search.provider", logActivity =false)</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>16</v>
@@ -1951,7 +1952,7 @@
       </c>
       <c r="L25" s="4"/>
       <c r="M25" t="str">
-        <f t="shared" ref="M25:M34" si="20">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D25,"','CONNON_CONFIG', 0, '",C25,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M25:M34" si="23">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D25,"','CONNON_CONFIG', 0, '",C25,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-02','CONNON_CONFIG', 0, 'Create Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N25" t="str">
@@ -1965,28 +1966,28 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="4" t="s">
@@ -1994,7 +1995,7 @@
       </c>
       <c r="L26" s="4"/>
       <c r="M26" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-03','CONNON_CONFIG', 0, 'Update Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N26" t="str">
@@ -2008,28 +2009,28 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="I27" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="4" t="s">
@@ -2037,7 +2038,7 @@
       </c>
       <c r="L27" s="4"/>
       <c r="M27" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-04','CONNON_CONFIG', 0, 'Update Post Status', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N27" t="str">
@@ -2051,28 +2052,28 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="4" t="s">
@@ -2080,7 +2081,7 @@
       </c>
       <c r="L28" s="4"/>
       <c r="M28" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-05','CONNON_CONFIG', 0, 'Delete Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N28" t="str">
@@ -2094,25 +2095,25 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>16</v>
@@ -2125,7 +2126,7 @@
       </c>
       <c r="L29" s="4"/>
       <c r="M29" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-06','CONNON_CONFIG', 0, 'Create Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N29" t="str">
@@ -2139,28 +2140,28 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="I30" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="4" t="s">
@@ -2168,7 +2169,7 @@
       </c>
       <c r="L30" s="4"/>
       <c r="M30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-07','CONNON_CONFIG', 0, 'Delete Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N30" t="str">
@@ -2182,25 +2183,25 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>16</v>
@@ -2211,7 +2212,7 @@
       </c>
       <c r="L31" s="4"/>
       <c r="M31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-08','CONNON_CONFIG', 0, 'Get Post Request Count', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N31" t="str">
@@ -2225,25 +2226,25 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>16</v>
@@ -2254,7 +2255,7 @@
       </c>
       <c r="L32" s="4"/>
       <c r="M32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-09','CONNON_CONFIG', 0, 'Get Post Request', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N32" t="str">
@@ -2268,25 +2269,25 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>16</v>
@@ -2297,39 +2298,39 @@
       </c>
       <c r="L33" s="4"/>
       <c r="M33" t="str">
-        <f t="shared" ref="M33" si="21">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D33,"','CONNON_CONFIG', 0, '",C33,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M33" si="24">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D33,"','CONNON_CONFIG', 0, '",C33,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-PS-10','CONNON_CONFIG', 0, 'Post Views', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" ref="N33" si="22">_xlfn.CONCAT(IF(I33="GET","@GetMapping(",IF(I33="POST","@PostMapping(",IF(I33="DELETE","@DeleteMapping(",IF(I33="PUT","@PutMapping(","")))),CHAR(34),H33,CHAR(34),")")</f>
+        <f t="shared" ref="N33" si="25">_xlfn.CONCAT(IF(I33="GET","@GetMapping(",IF(I33="POST","@PostMapping(",IF(I33="DELETE","@DeleteMapping(",IF(I33="PUT","@PutMapping(","")))),CHAR(34),H33,CHAR(34),")")</f>
         <v>@PostMapping("/views")</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" ref="O33" si="23">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D33,,CHAR(34),", serviceName = ",CHAR(34),C33,CHAR(34), ", queryId = ",CHAR(34),E33,CHAR(34),", logActivity =",F33,")")</f>
+        <f t="shared" ref="O33" si="26">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D33,,CHAR(34),", serviceName = ",CHAR(34),C33,CHAR(34), ", queryId = ",CHAR(34),E33,CHAR(34),", logActivity =",F33,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-PS-10", serviceName = "Post Views", queryId = "app.post.save.viewe", logActivity =false)</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="F34" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="H34" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>16</v>
@@ -2338,7 +2339,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-SP-01','CONNON_CONFIG', 0, 'Search Service Provider For Post', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N34" t="str">
@@ -2352,23 +2353,23 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>16</v>
@@ -2377,37 +2378,37 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" t="str">
-        <f t="shared" ref="M35" si="24">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D35,"','CONNON_CONFIG', 0, '",C35,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M35" si="27">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D35,"','CONNON_CONFIG', 0, '",C35,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-FL-01','CONNON_CONFIG', 0, 'File Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" ref="N35" si="25">_xlfn.CONCAT(IF(I35="GET","@GetMapping(",IF(I35="POST","@PostMapping(",IF(I35="DELETE","@DeleteMapping(",IF(I35="PUT","@PutMapping(","")))),CHAR(34),H35,CHAR(34),")")</f>
+        <f t="shared" ref="N35" si="28">_xlfn.CONCAT(IF(I35="GET","@GetMapping(",IF(I35="POST","@PostMapping(",IF(I35="DELETE","@DeleteMapping(",IF(I35="PUT","@PutMapping(","")))),CHAR(34),H35,CHAR(34),")")</f>
         <v>@PostMapping("/fileupload")</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" ref="O35" si="26">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D35,,CHAR(34),", serviceName = ",CHAR(34),C35,CHAR(34), ", queryId = ",CHAR(34),E35,CHAR(34),", logActivity =",F35,")")</f>
+        <f t="shared" ref="O35" si="29">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D35,,CHAR(34),", serviceName = ",CHAR(34),C35,CHAR(34), ", queryId = ",CHAR(34),E35,CHAR(34),", logActivity =",F35,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-FL-01", serviceName = "File Upload", queryId = "", logActivity =false)</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>16</v>
@@ -2418,39 +2419,39 @@
       </c>
       <c r="L36" s="4"/>
       <c r="M36" t="str">
-        <f t="shared" ref="M36" si="27">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D36,"','CONNON_CONFIG', 0, '",C36,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M36" si="30">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D36,"','CONNON_CONFIG', 0, '",C36,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-IMG-01','CONNON_CONFIG', 0, 'Image Upload', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" ref="N36" si="28">_xlfn.CONCAT(IF(I36="GET","@GetMapping(",IF(I36="POST","@PostMapping(",IF(I36="DELETE","@DeleteMapping(",IF(I36="PUT","@PutMapping(","")))),CHAR(34),H36,CHAR(34),")")</f>
+        <f t="shared" ref="N36" si="31">_xlfn.CONCAT(IF(I36="GET","@GetMapping(",IF(I36="POST","@PostMapping(",IF(I36="DELETE","@DeleteMapping(",IF(I36="PUT","@PutMapping(","")))),CHAR(34),H36,CHAR(34),")")</f>
         <v>@PostMapping("/image")</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" ref="O36" si="29">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D36,,CHAR(34),", serviceName = ",CHAR(34),C36,CHAR(34), ", queryId = ",CHAR(34),E36,CHAR(34),", logActivity =",F36,")")</f>
+        <f t="shared" ref="O36" si="32">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D36,,CHAR(34),", serviceName = ",CHAR(34),C36,CHAR(34), ", queryId = ",CHAR(34),E36,CHAR(34),", logActivity =",F36,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-IMG-01", serviceName = "Image Upload", queryId = "", logActivity =false)</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="F37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="H37" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>16</v>
@@ -2461,15 +2462,15 @@
       </c>
       <c r="L37" s="4"/>
       <c r="M37" t="str">
-        <f t="shared" ref="M37" si="30">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D37,"','CONNON_CONFIG', 0, '",C37,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <f t="shared" ref="M37" si="33">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D37,"','CONNON_CONFIG', 0, '",C37,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
         <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-BID-01','CONNON_CONFIG', 0, 'Create Post bid', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" ref="N37" si="31">_xlfn.CONCAT(IF(I37="GET","@GetMapping(",IF(I37="POST","@PostMapping(",IF(I37="DELETE","@DeleteMapping(",IF(I37="PUT","@PutMapping(","")))),CHAR(34),H37,CHAR(34),")")</f>
+        <f t="shared" ref="N37" si="34">_xlfn.CONCAT(IF(I37="GET","@GetMapping(",IF(I37="POST","@PostMapping(",IF(I37="DELETE","@DeleteMapping(",IF(I37="PUT","@PutMapping(","")))),CHAR(34),H37,CHAR(34),")")</f>
         <v>@PostMapping("/create")</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" ref="O37" si="32">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D37,,CHAR(34),", serviceName = ",CHAR(34),C37,CHAR(34), ", queryId = ",CHAR(34),E37,CHAR(34),", logActivity =",F37,")")</f>
+        <f t="shared" ref="O37" si="35">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D37,,CHAR(34),", serviceName = ",CHAR(34),C37,CHAR(34), ", queryId = ",CHAR(34),E37,CHAR(34),", logActivity =",F37,")")</f>
         <v>@ServiceInfo(serviceCode = "WS-BID-01", serviceName = "Create Post bid", queryId = "app.bid.post.insert", logActivity =true)</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feedback form basic layout
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C543655-687E-8F45-B892-3129077E5A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E221508-1559-484D-93C5-EA19C6B2563E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="170">
   <si>
     <t>Services</t>
   </si>
@@ -523,6 +523,21 @@
   </si>
   <si>
     <t>/setnewpassword</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>WS-FED-01</t>
+  </si>
+  <si>
+    <t>app.feedback.question.get</t>
+  </si>
+  <si>
+    <t>Get feedback Question</t>
+  </si>
+  <si>
+    <t>/getquestion</t>
   </si>
 </sst>
 </file>
@@ -932,11 +947,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
-  <dimension ref="B3:O37"/>
+  <dimension ref="B3:O38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2474,6 +2489,47 @@
         <v>@ServiceInfo(serviceCode = "WS-BID-01", serviceName = "Create Post bid", queryId = "app.bid.post.insert", logActivity =true)</v>
       </c>
     </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" t="str">
+        <f t="shared" ref="M38" si="36">_xlfn.CONCAT("INSERT INTO ",CHAR(34),"M_CTL_CONFIG",CHAR(34)," VALUES('",D38,"','CONNON_CONFIG', 0, '",C38,"', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);")</f>
+        <v>INSERT INTO "M_CTL_CONFIG" VALUES('WS-FED-01','CONNON_CONFIG', 0, 'Get feedback Question', '{}', 0, 0, CURRENT_TIMESTAMP, 'ATUL', null, null);</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" ref="N38" si="37">_xlfn.CONCAT(IF(I38="GET","@GetMapping(",IF(I38="POST","@PostMapping(",IF(I38="DELETE","@DeleteMapping(",IF(I38="PUT","@PutMapping(","")))),CHAR(34),H38,CHAR(34),")")</f>
+        <v>@PostMapping("/getquestion")</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" ref="O38" si="38">_xlfn.CONCAT("@ServiceInfo(serviceCode = ",CHAR(34),D38,,CHAR(34),", serviceName = ",CHAR(34),C38,CHAR(34), ", queryId = ",CHAR(34),E38,CHAR(34),", logActivity =",F38,")")</f>
+        <v>@ServiceInfo(serviceCode = "WS-FED-01", serviceName = "Get feedback Question", queryId = "app.feedback.question.get", logActivity =false)</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B3:L35" xr:uid="{B873333A-9513-0D4B-818E-F6CEEC3D4866}"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Vehicle screen changes and icon changes.
</commit_message>
<xml_diff>
--- a/Documents/Services/ServicesList.xlsx
+++ b/Documents/Services/ServicesList.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0684218D-B798-594C-8B0C-1C3FB0AE7F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A40E22F-9586-AA49-8E6C-3B960EA33AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" activeTab="1" xr2:uid="{EFF1F141-FA33-0340-81EC-DEEEED813790}"/>
   </bookViews>
   <sheets>
     <sheet name="ServicesList" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ServicesList!$B$3:$L$35</definedName>
@@ -22,6 +23,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -973,9 +981,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687EB0A-3A46-424E-8B7E-E4D7D7758F41}">
   <dimension ref="B3:O40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N40" sqref="N40:O40"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2641,4 +2649,48 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1DB4946-81CA-3247-B775-0AAAC5882CAD}">
+  <dimension ref="D3:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <f>E4*30</f>
+        <v>30000</v>
+      </c>
+      <c r="G4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f>G4*12</f>
+        <v>60000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>